<commit_message>
ux preset view & aci app update
</commit_message>
<xml_diff>
--- a/application/aci/locale.xlsx
+++ b/application/aci/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="183">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -469,6 +469,277 @@
   </si>
   <si>
     <t>인터페이스 포트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bridge Domain Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브릿지도메인 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Application Profile Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로파일 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bridge Domain Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브릿지도메인 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서브넷 주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subnet IP</t>
+  </si>
+  <si>
+    <t>Context Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VRF 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VRF 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contract Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트랙 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contract Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트랙 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필터 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필터 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L3 External Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외부네트워크 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L3 External Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외부네트워크 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter Entry Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter Entry Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필터 엔트리 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필터 엔트리 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서브젝트 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subject Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refresh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태점수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보갱신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tenant Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테넌트 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장치 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EPG Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>망분리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할당경로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Binding Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이용계약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제공계약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔드포인트그룹 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Endpoint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔드포인트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연관정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브릿지도메인 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumed Contracts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bridge Domain Relations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Provided Contracts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Path Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경로 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경로 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Path Attachments</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재상태수치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Endpoint Group Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔드포인트그룹 상태정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 상태정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노드 상태정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -842,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1597,6 +1868,496 @@
         <v>114</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Arrange for Excel & Add Acl Logging
</commit_message>
<xml_diff>
--- a/application/aci/locale.xlsx
+++ b/application/aci/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="312">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1224,6 +1224,38 @@
   </si>
   <si>
     <t>DN 또는 Class 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출발지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Destination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도착지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Protocol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로토콜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>길이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1597,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3752,6 +3784,62 @@
         <v>269</v>
       </c>
     </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D153">
     <sortCondition ref="A2:A153"/>

</xml_diff>

<commit_message>
Stable Release for KRIHS
</commit_message>
<xml_diff>
--- a/application/aci/locale.xlsx
+++ b/application/aci/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="332">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1320,6 +1320,22 @@
   </si>
   <si>
     <t>오브젝트 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count Table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeStamp Table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간 기록 테이블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>합계 테이블</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1693,10 +1709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:D166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2296,584 +2312,584 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>196</v>
+        <v>328</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>196</v>
+        <v>328</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>197</v>
+        <v>331</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>197</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>265</v>
+        <v>210</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>265</v>
+        <v>210</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>270</v>
+        <v>211</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>270</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>142</v>
+        <v>265</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>142</v>
+        <v>265</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>143</v>
+        <v>270</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>143</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>274</v>
+        <v>142</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>274</v>
+        <v>142</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>276</v>
+        <v>143</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>276</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>203</v>
+        <v>276</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>203</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>307</v>
+        <v>232</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>307</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>61</v>
+        <v>306</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>306</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>62</v>
+        <v>307</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>63</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>122</v>
+        <v>61</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>8</v>
+        <v>122</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>242</v>
+        <v>7</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>243</v>
+        <v>10</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>243</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>302</v>
+        <v>242</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>302</v>
+        <v>242</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>303</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>38</v>
+        <v>302</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>39</v>
+        <v>303</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>39</v>
+        <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>323</v>
+        <v>25</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>324</v>
+        <v>26</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>324</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>124</v>
+        <v>323</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>124</v>
+        <v>323</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>125</v>
+        <v>324</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>125</v>
+        <v>324</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>229</v>
+        <v>147</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>229</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>43</v>
+        <v>241</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>296</v>
+        <v>43</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>300</v>
+        <v>44</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>300</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>83</v>
+        <v>296</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>84</v>
+        <v>300</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>84</v>
+        <v>300</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>277</v>
+        <v>15</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>278</v>
+        <v>16</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>278</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>221</v>
+        <v>278</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>221</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>194</v>
+        <v>262</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>194</v>
+        <v>262</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>50</v>
+        <v>194</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>51</v>
+        <v>195</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>51</v>
+        <v>195</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>106</v>
+        <v>50</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>219</v>
+        <v>104</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>219</v>
+        <v>104</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>223</v>
+        <v>105</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>223</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>289</v>
+        <v>219</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>289</v>
+        <v>219</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>288</v>
+        <v>223</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>288</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>118</v>
+        <v>281</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>118</v>
+        <v>281</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>183</v>
@@ -2884,276 +2900,276 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>56</v>
+        <v>180</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>198</v>
+        <v>56</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>199</v>
+        <v>73</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>199</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>17</v>
+        <v>204</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>321</v>
+        <v>13</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>322</v>
+        <v>14</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>322</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>154</v>
+        <v>321</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>321</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>155</v>
+        <v>322</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>155</v>
+        <v>322</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>233</v>
+        <v>156</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>233</v>
+        <v>156</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>79</v>
+        <v>217</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>79</v>
+        <v>217</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>81</v>
+        <v>221</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>81</v>
+        <v>221</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>310</v>
+        <v>79</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>310</v>
+        <v>79</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>311</v>
+        <v>81</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>311</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>130</v>
+        <v>295</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>130</v>
+        <v>295</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>266</v>
+        <v>130</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>271</v>
+        <v>130</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>181</v>
+        <v>244</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>181</v>
+        <v>244</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>184</v>
@@ -3164,80 +3180,80 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>297</v>
+        <v>192</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>297</v>
+        <v>192</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>301</v>
+        <v>193</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>301</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>272</v>
+        <v>301</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>272</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>187</v>
+        <v>291</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>187</v>
+        <v>291</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>189</v>
+        <v>293</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>189</v>
+        <v>293</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>189</v>
@@ -3248,763 +3264,791 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>170</v>
+        <v>188</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>240</v>
+        <v>170</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>40</v>
+        <v>145</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>41</v>
+        <v>149</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>41</v>
+        <v>149</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>283</v>
+        <v>40</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>150</v>
+        <v>283</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>74</v>
+        <v>327</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>74</v>
+        <v>326</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>286</v>
+        <v>150</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>287</v>
+        <v>152</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>287</v>
+        <v>152</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>284</v>
+        <v>57</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>284</v>
+        <v>57</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>285</v>
+        <v>74</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>285</v>
+        <v>74</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>141</v>
+        <v>286</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>141</v>
+        <v>286</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>139</v>
+        <v>284</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>139</v>
+        <v>284</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>140</v>
+        <v>285</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>140</v>
+        <v>285</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>246</v>
+        <v>141</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>246</v>
+        <v>141</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>87</v>
+        <v>294</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>157</v>
+        <v>298</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>157</v>
+        <v>298</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>185</v>
+        <v>87</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>308</v>
+        <v>175</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>308</v>
+        <v>175</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>309</v>
+        <v>157</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>309</v>
+        <v>157</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>253</v>
+        <v>138</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>253</v>
+        <v>138</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>258</v>
+        <v>129</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>258</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>27</v>
+        <v>253</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>133</v>
+        <v>255</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>133</v>
+        <v>255</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>134</v>
+        <v>259</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>134</v>
+        <v>259</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>11</v>
+        <v>133</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>304</v>
+        <v>54</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>304</v>
+        <v>54</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>305</v>
+        <v>55</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>305</v>
+        <v>55</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>117</v>
+        <v>304</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>116</v>
+        <v>305</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>116</v>
+        <v>305</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>252</v>
+        <v>77</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>225</v>
+        <v>80</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>225</v>
+        <v>80</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>208</v>
+        <v>95</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>208</v>
+        <v>95</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>209</v>
+        <v>94</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>209</v>
+        <v>94</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>70</v>
+        <v>206</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>71</v>
+        <v>207</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>72</v>
+        <v>207</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>263</v>
+        <v>120</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>263</v>
+        <v>120</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>264</v>
+        <v>121</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>264</v>
+        <v>121</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>168</v>
+        <v>70</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>169</v>
+        <v>72</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>317</v>
+        <v>263</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>317</v>
+        <v>263</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>319</v>
+        <v>264</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>319</v>
+        <v>264</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>144</v>
+        <v>329</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>144</v>
+        <v>329</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>148</v>
+        <v>330</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>148</v>
+        <v>330</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>316</v>
+        <v>168</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>316</v>
+        <v>168</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>320</v>
+        <v>169</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>318</v>
+        <v>169</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>312</v>
+        <v>144</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>312</v>
+        <v>144</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>314</v>
+        <v>148</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>314</v>
+        <v>148</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>28</v>
+        <v>313</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>313</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>29</v>
+        <v>315</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>29</v>
+        <v>315</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>59</v>
+        <v>312</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>312</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>60</v>
+        <v>314</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>60</v>
+        <v>314</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>162</v>
+        <v>290</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>162</v>
+        <v>290</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>163</v>
+        <v>292</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>163</v>
+        <v>292</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>172</v>
+        <v>28</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>174</v>
+        <v>29</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>174</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>176</v>
+        <v>58</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>268</v>
+        <v>172</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>269</v>
+        <v>174</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>269</v>
+        <v>174</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>325</v>
+        <v>176</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>325</v>
+        <v>176</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>327</v>
+        <v>178</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>326</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D163">
-    <sortCondition ref="A2:A163"/>
+  <sortState ref="A2:D166">
+    <sortCondition ref="A2:A166"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pretty Update & Hanjin
</commit_message>
<xml_diff>
--- a/application/aci/locale.xlsx
+++ b/application/aci/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="336">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1336,6 +1336,22 @@
   </si>
   <si>
     <t>합계 테이블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active Interfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인터페이스 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active Endpoints</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔드포인트 상태</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1709,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D166"/>
+  <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1892,2163 +1908,2191 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>334</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>335</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>332</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>333</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>90</v>
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>66</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>212</v>
+        <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>212</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>213</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>213</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>127</v>
+        <v>85</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>212</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>88</v>
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>214</v>
+        <v>88</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>214</v>
+        <v>88</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>215</v>
+        <v>89</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>215</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>214</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>215</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>136</v>
+        <v>5</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>249</v>
+        <v>3</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>251</v>
+        <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>251</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>254</v>
+        <v>136</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>254</v>
+        <v>136</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>257</v>
+        <v>128</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>257</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>48</v>
+        <v>254</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>49</v>
+        <v>257</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>49</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>98</v>
+        <v>256</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>98</v>
+        <v>256</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>96</v>
+        <v>48</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>216</v>
+        <v>98</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>216</v>
+        <v>98</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>218</v>
+        <v>100</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>218</v>
+        <v>100</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>222</v>
+        <v>101</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>222</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>328</v>
+        <v>218</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>328</v>
+        <v>218</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>331</v>
+        <v>222</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>331</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>196</v>
+        <v>75</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>196</v>
+        <v>75</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>197</v>
+        <v>76</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>197</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>210</v>
+        <v>328</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>210</v>
+        <v>328</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>211</v>
+        <v>331</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>211</v>
+        <v>331</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>265</v>
+        <v>196</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>265</v>
+        <v>196</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>270</v>
+        <v>197</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>270</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>202</v>
+        <v>142</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>202</v>
+        <v>142</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>232</v>
+        <v>276</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>232</v>
+        <v>276</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>306</v>
+        <v>202</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>306</v>
+        <v>202</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>307</v>
+        <v>203</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>307</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>61</v>
+        <v>231</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>63</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>122</v>
+        <v>306</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>122</v>
+        <v>306</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>123</v>
+        <v>307</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>123</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>7</v>
+        <v>122</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>242</v>
+        <v>8</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>243</v>
+        <v>9</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>243</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>302</v>
+        <v>7</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>303</v>
+        <v>10</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>303</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>38</v>
+        <v>242</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>25</v>
+        <v>302</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>26</v>
+        <v>303</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>26</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>323</v>
+        <v>38</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>324</v>
+        <v>39</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>324</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>124</v>
+        <v>25</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>131</v>
+        <v>323</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>131</v>
+        <v>323</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>132</v>
+        <v>324</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>132</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>241</v>
+        <v>131</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>241</v>
+        <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>229</v>
+        <v>132</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>229</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>296</v>
+        <v>241</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>296</v>
+        <v>241</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>15</v>
+        <v>296</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>16</v>
+        <v>300</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>16</v>
+        <v>300</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>277</v>
+        <v>83</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>278</v>
+        <v>84</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>278</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>262</v>
+        <v>15</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>221</v>
+        <v>16</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>221</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>194</v>
+        <v>277</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>194</v>
+        <v>277</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>195</v>
+        <v>278</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>195</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>50</v>
+        <v>262</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>51</v>
+        <v>221</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>51</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>106</v>
+        <v>194</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>106</v>
+        <v>194</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>107</v>
+        <v>195</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>107</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>113</v>
+        <v>50</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>219</v>
+        <v>112</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>219</v>
+        <v>112</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>223</v>
+        <v>115</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>223</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>288</v>
+        <v>105</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>288</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>273</v>
+        <v>219</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>273</v>
+        <v>219</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>275</v>
+        <v>223</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>275</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>119</v>
+        <v>275</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>119</v>
+        <v>275</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>167</v>
+        <v>281</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>167</v>
+        <v>281</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>166</v>
+        <v>282</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>166</v>
+        <v>282</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>56</v>
+        <v>179</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>204</v>
+        <v>56</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>205</v>
+        <v>73</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>205</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>17</v>
+        <v>198</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>13</v>
+        <v>204</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>14</v>
+        <v>205</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>14</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>321</v>
+        <v>17</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>154</v>
+        <v>13</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>156</v>
+        <v>321</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>156</v>
+        <v>321</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>157</v>
+        <v>322</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>157</v>
+        <v>322</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>233</v>
+        <v>153</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>234</v>
+        <v>155</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>234</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>108</v>
+        <v>233</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>108</v>
+        <v>233</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>109</v>
+        <v>234</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>109</v>
+        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>217</v>
+        <v>110</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>217</v>
+        <v>110</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>221</v>
+        <v>111</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>221</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>311</v>
+        <v>221</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>311</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>295</v>
+        <v>79</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>295</v>
+        <v>79</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>299</v>
+        <v>81</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>299</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>130</v>
+        <v>310</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>130</v>
+        <v>310</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>266</v>
+        <v>295</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>266</v>
+        <v>295</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>244</v>
+        <v>130</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>245</v>
+        <v>130</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>181</v>
+        <v>266</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>181</v>
+        <v>266</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>184</v>
+        <v>271</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>184</v>
+        <v>271</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>297</v>
+        <v>182</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>297</v>
+        <v>182</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>301</v>
+        <v>184</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>301</v>
+        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>267</v>
+        <v>192</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>267</v>
+        <v>192</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>272</v>
+        <v>193</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>272</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>187</v>
+        <v>267</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>187</v>
+        <v>267</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>189</v>
+        <v>272</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>189</v>
+        <v>272</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>188</v>
+        <v>291</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>188</v>
+        <v>291</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>189</v>
+        <v>293</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>189</v>
+        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>170</v>
+        <v>187</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>240</v>
+        <v>188</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>240</v>
+        <v>188</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>145</v>
+        <v>170</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>40</v>
+        <v>240</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>283</v>
+        <v>145</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>283</v>
+        <v>145</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>325</v>
+        <v>40</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>327</v>
+        <v>41</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>326</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>150</v>
+        <v>283</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>74</v>
+        <v>327</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>74</v>
+        <v>326</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>286</v>
+        <v>150</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>287</v>
+        <v>152</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>287</v>
+        <v>152</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>284</v>
+        <v>57</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>284</v>
+        <v>57</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>285</v>
+        <v>74</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>285</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>141</v>
+        <v>286</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>141</v>
+        <v>286</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>139</v>
+        <v>284</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>139</v>
+        <v>284</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>140</v>
+        <v>285</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>140</v>
+        <v>285</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>246</v>
+        <v>141</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>246</v>
+        <v>141</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>87</v>
+        <v>294</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>157</v>
+        <v>298</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>157</v>
+        <v>298</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>185</v>
+        <v>87</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>308</v>
+        <v>175</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>308</v>
+        <v>175</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>309</v>
+        <v>157</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>309</v>
+        <v>157</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>253</v>
+        <v>138</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>253</v>
+        <v>138</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>258</v>
+        <v>129</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>258</v>
+        <v>129</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>27</v>
+        <v>253</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>42</v>
+        <v>258</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>133</v>
+        <v>255</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>133</v>
+        <v>255</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>134</v>
+        <v>259</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>134</v>
+        <v>259</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>11</v>
+        <v>133</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>304</v>
+        <v>54</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>304</v>
+        <v>54</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>305</v>
+        <v>55</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>305</v>
+        <v>55</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>117</v>
+        <v>304</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>116</v>
+        <v>305</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>116</v>
+        <v>305</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>252</v>
+        <v>77</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>225</v>
+        <v>80</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>225</v>
+        <v>80</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>208</v>
+        <v>95</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>208</v>
+        <v>95</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>209</v>
+        <v>94</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>209</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>70</v>
+        <v>206</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>71</v>
+        <v>207</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>72</v>
+        <v>207</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>263</v>
+        <v>120</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>263</v>
+        <v>120</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>264</v>
+        <v>121</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>264</v>
+        <v>121</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>329</v>
+        <v>70</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>330</v>
+        <v>71</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>330</v>
+        <v>72</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>168</v>
+        <v>263</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>168</v>
+        <v>263</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>169</v>
+        <v>264</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>169</v>
+        <v>264</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>313</v>
+        <v>144</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>313</v>
+        <v>144</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>315</v>
+        <v>148</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>315</v>
+        <v>148</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>28</v>
+        <v>312</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>312</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>29</v>
+        <v>314</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>29</v>
+        <v>314</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>59</v>
+        <v>290</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>60</v>
+        <v>292</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>60</v>
+        <v>292</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>162</v>
+        <v>28</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>172</v>
+        <v>58</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B168" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C168" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D166" s="2" t="s">
+      <c r="D168" s="2" t="s">
         <v>269</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D166">
-    <sortCondition ref="A2:A166"/>
+  <sortState ref="A2:D168">
+    <sortCondition ref="A2:A168"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pretty update & layout fix
</commit_message>
<xml_diff>
--- a/application/aci/locale.xlsx
+++ b/application/aci/locale.xlsx
@@ -1351,7 +1351,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>엔드포인트 상태</t>
+    <t>등록된 엔드포인트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1727,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add IP Mobility on EPG
</commit_message>
<xml_diff>
--- a/application/aci/locale.xlsx
+++ b/application/aci/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="354">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1352,6 +1352,78 @@
   </si>
   <si>
     <t>등록된 엔드포인트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP Mobility</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP 모빌리티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register IPs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP(구간) 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register IPs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mobility IPs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP 모빌리티 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP Start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작 IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작 IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP End</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP End</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종료 IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종료 IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부가설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use EPG Subnet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EPG 서브넷 사용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1725,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4090,6 +4162,104 @@
         <v>269</v>
       </c>
     </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D168">
     <sortCondition ref="A2:A168"/>

</xml_diff>